<commit_message>
Updated map and shop
</commit_message>
<xml_diff>
--- a/Design and Narrative/Shop.xlsx
+++ b/Design and Narrative/Shop.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>EATABLES</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Weapon 5</t>
   </si>
   <si>
-    <t>COIN Drops</t>
-  </si>
-  <si>
     <t>Small enemy</t>
   </si>
   <si>
@@ -94,13 +91,28 @@
     <t>( -1 every 1 secs after the initial boost)</t>
   </si>
   <si>
-    <t>Hunger (health depletion)</t>
-  </si>
-  <si>
     <t>Coins</t>
   </si>
   <si>
-    <t>Health decrease per hit from enemy</t>
+    <t>Hunger recovery</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotten Meat </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hunger </t>
+  </si>
+  <si>
+    <t>ENEMIES</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Game Start</t>
   </si>
 </sst>
 </file>
@@ -162,25 +174,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -487,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:S10"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -500,6 +515,7 @@
     <col min="4" max="4" width="16.109375" customWidth="1"/>
     <col min="7" max="7" width="15.109375" customWidth="1"/>
     <col min="9" max="9" width="11.21875" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" customWidth="1"/>
     <col min="15" max="15" width="11.88671875" customWidth="1"/>
     <col min="16" max="16" width="17.88671875" customWidth="1"/>
     <col min="17" max="17" width="12.6640625" customWidth="1"/>
@@ -507,75 +523,88 @@
     <col min="20" max="20" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2">
-        <v>100</v>
-      </c>
-      <c r="G2" s="1" t="s">
+        <v>10000</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="O2" s="3" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="O2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>5000</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="O3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+    </row>
+    <row r="4" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>200</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="O3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-    </row>
-    <row r="4" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="G4" s="2" t="s">
+      <c r="J4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="6"/>
-      <c r="O4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
     </row>
     <row r="5" spans="1:19" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G5" t="s">
@@ -585,12 +614,15 @@
         <v>10</v>
       </c>
       <c r="I5">
+        <v>20</v>
+      </c>
+      <c r="J5">
         <v>5</v>
       </c>
       <c r="O5" t="s">
         <v>12</v>
       </c>
-      <c r="P5" s="7" t="s">
+      <c r="P5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="Q5">
@@ -599,7 +631,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -610,6 +642,9 @@
         <v>12</v>
       </c>
       <c r="I6">
+        <v>22</v>
+      </c>
+      <c r="J6">
         <v>7</v>
       </c>
       <c r="O6" t="s">
@@ -622,12 +657,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>28</v>
+    <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>11</v>
       </c>
       <c r="G7" t="s">
         <v>6</v>
@@ -636,6 +674,9 @@
         <v>25</v>
       </c>
       <c r="I7">
+        <v>30</v>
+      </c>
+      <c r="J7">
         <v>12</v>
       </c>
       <c r="O7" t="s">
@@ -649,14 +690,17 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>19</v>
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>3000</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="D8">
-        <v>-2</v>
+        <v>20</v>
       </c>
       <c r="G8" t="s">
         <v>7</v>
@@ -665,6 +709,9 @@
         <v>50</v>
       </c>
       <c r="I8">
+        <v>45</v>
+      </c>
+      <c r="J8">
         <v>30</v>
       </c>
       <c r="O8" t="s">
@@ -678,14 +725,17 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>20</v>
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <v>5000</v>
       </c>
       <c r="C9">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="D9">
-        <v>-5</v>
+        <v>50</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
@@ -694,13 +744,13 @@
         <v>30</v>
       </c>
       <c r="I9">
+        <v>35</v>
+      </c>
+      <c r="J9">
         <v>25</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>-1</v>
-      </c>
-      <c r="K9" t="s">
-        <v>25</v>
       </c>
       <c r="O9" t="s">
         <v>17</v>
@@ -713,14 +763,30 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>21</v>
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>7000</v>
       </c>
       <c r="C10">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D10">
-        <v>-10</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on coins drops & enemy damage in Shop
</commit_message>
<xml_diff>
--- a/Design and Narrative/Shop.xlsx
+++ b/Design and Narrative/Shop.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Enemies" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
   <si>
     <t>EATABLES</t>
   </si>
@@ -58,27 +59,6 @@
     <t>player already has at game begeinning</t>
   </si>
   <si>
-    <t>Weapon 2</t>
-  </si>
-  <si>
-    <t>Weapon 3</t>
-  </si>
-  <si>
-    <t>Weapon 4</t>
-  </si>
-  <si>
-    <t>Weapon 5</t>
-  </si>
-  <si>
-    <t>Small enemy</t>
-  </si>
-  <si>
-    <t>Medium enemy</t>
-  </si>
-  <si>
-    <t>Large enemy</t>
-  </si>
-  <si>
     <t>Heath recovered</t>
   </si>
   <si>
@@ -88,9 +68,6 @@
     <t>Health depletion</t>
   </si>
   <si>
-    <t>( -1 every 1 secs after the initial boost)</t>
-  </si>
-  <si>
     <t>Coins</t>
   </si>
   <si>
@@ -113,6 +90,90 @@
   </si>
   <si>
     <t>Game Start</t>
+  </si>
+  <si>
+    <t>Zombie</t>
+  </si>
+  <si>
+    <t>Titans</t>
+  </si>
+  <si>
+    <t>Dragonswasps</t>
+  </si>
+  <si>
+    <t>Wormers</t>
+  </si>
+  <si>
+    <t>Small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium </t>
+  </si>
+  <si>
+    <t>Large</t>
+  </si>
+  <si>
+    <t>Kebab</t>
+  </si>
+  <si>
+    <t>Lemonade</t>
+  </si>
+  <si>
+    <t>Shotgun</t>
+  </si>
+  <si>
+    <t>Machine Gun</t>
+  </si>
+  <si>
+    <t>Sniper Rifle</t>
+  </si>
+  <si>
+    <t>Bomb</t>
+  </si>
+  <si>
+    <t>( -5 every 1 secs after the initial boost)</t>
+  </si>
+  <si>
+    <t>(10 health recovery every 5 sec)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wave 1 </t>
+  </si>
+  <si>
+    <t>small</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>large</t>
+  </si>
+  <si>
+    <t>Dragonwasps</t>
+  </si>
+  <si>
+    <t>Coins earned</t>
+  </si>
+  <si>
+    <t>Wave 2</t>
+  </si>
+  <si>
+    <t>Wave 3</t>
+  </si>
+  <si>
+    <t>Wave 4</t>
+  </si>
+  <si>
+    <t>Wave 5</t>
+  </si>
+  <si>
+    <t>Wave 6</t>
+  </si>
+  <si>
+    <t>Wave 7</t>
+  </si>
+  <si>
+    <t>Damage Taken</t>
   </si>
 </sst>
 </file>
@@ -174,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -183,6 +244,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -194,8 +259,14 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -504,15 +575,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.44140625" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" customWidth="1"/>
     <col min="7" max="7" width="15.109375" customWidth="1"/>
     <col min="9" max="9" width="11.21875" customWidth="1"/>
     <col min="10" max="10" width="10.6640625" customWidth="1"/>
@@ -525,59 +597,62 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>10000</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="C2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="O2" s="7" t="s">
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="O2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B3">
         <v>5000</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="O3" s="7" t="s">
+      <c r="G3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="O3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
     </row>
     <row r="4" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B4">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>2</v>
@@ -586,13 +661,13 @@
         <v>3</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>2</v>
@@ -608,16 +683,16 @@
     </row>
     <row r="5" spans="1:19" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I5">
         <v>20</v>
       </c>
       <c r="J5">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="O5" t="s">
         <v>12</v>
@@ -630,25 +705,20 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B6" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
       <c r="G6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H6">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="I6">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="J6">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="O6" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="P6">
         <v>50</v>
@@ -658,29 +728,20 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>11</v>
-      </c>
       <c r="G7" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="H7">
         <v>25</v>
       </c>
       <c r="I7">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J7">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="O7" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="P7">
         <v>75</v>
@@ -690,32 +751,20 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8">
-        <v>3000</v>
-      </c>
-      <c r="C8">
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <v>35</v>
+      </c>
+      <c r="I8">
         <v>50</v>
       </c>
-      <c r="D8">
-        <v>20</v>
-      </c>
-      <c r="G8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8">
-        <v>50</v>
-      </c>
-      <c r="I8">
-        <v>45</v>
-      </c>
       <c r="J8">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="P8">
         <v>100</v>
@@ -725,35 +774,23 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9">
-        <v>5000</v>
-      </c>
-      <c r="C9">
-        <v>80</v>
-      </c>
-      <c r="D9">
-        <v>50</v>
-      </c>
       <c r="G9" t="s">
         <v>8</v>
       </c>
       <c r="H9">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="I9">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="J9">
-        <v>25</v>
+        <v>150</v>
       </c>
       <c r="K9">
-        <v>-1</v>
+        <v>-5</v>
       </c>
       <c r="O9" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="P9">
         <v>120</v>
@@ -763,39 +800,525 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10">
-        <v>7000</v>
-      </c>
-      <c r="C10">
+      <c r="G10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10">
+        <v>60</v>
+      </c>
+      <c r="I10">
+        <v>80</v>
+      </c>
+      <c r="J10">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11">
+        <v>120</v>
+      </c>
+      <c r="I11">
         <v>100</v>
       </c>
-      <c r="D10">
-        <v>100</v>
+      <c r="J11">
+        <v>500</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <sortState ref="G5:K11">
+    <sortCondition ref="H19"/>
+  </sortState>
+  <mergeCells count="4">
     <mergeCell ref="G3:K3"/>
     <mergeCell ref="O3:S3"/>
     <mergeCell ref="G2:K2"/>
     <mergeCell ref="O2:S2"/>
-    <mergeCell ref="B6:D6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:P31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" customWidth="1"/>
+    <col min="9" max="9" width="17.77734375" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" customWidth="1"/>
+    <col min="12" max="12" width="11.77734375" customWidth="1"/>
+    <col min="13" max="13" width="12.21875" customWidth="1"/>
+    <col min="14" max="14" width="12.5546875" customWidth="1"/>
+    <col min="15" max="15" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="H4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+    </row>
+    <row r="5" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="H5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F6" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6">
+        <v>3000</v>
+      </c>
+      <c r="I6">
+        <v>50</v>
+      </c>
+      <c r="J6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F7" s="11"/>
+      <c r="G7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7">
+        <v>5000</v>
+      </c>
+      <c r="I7">
+        <v>80</v>
+      </c>
+      <c r="J7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F8" s="11"/>
+      <c r="G8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8">
+        <v>7000</v>
+      </c>
+      <c r="I8">
+        <v>100</v>
+      </c>
+      <c r="J8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9">
+        <v>4000</v>
+      </c>
+      <c r="I9">
+        <v>60</v>
+      </c>
+      <c r="J9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F10" s="11"/>
+      <c r="G10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10">
+        <v>6000</v>
+      </c>
+      <c r="I10">
+        <v>90</v>
+      </c>
+      <c r="J10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F11" s="11"/>
+      <c r="G11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11">
+        <v>8000</v>
+      </c>
+      <c r="I11">
+        <v>110</v>
+      </c>
+      <c r="J11">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12">
+        <v>5000</v>
+      </c>
+      <c r="I12">
+        <v>70</v>
+      </c>
+      <c r="J12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F13" s="11"/>
+      <c r="G13" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13">
+        <v>7000</v>
+      </c>
+      <c r="I13">
+        <v>100</v>
+      </c>
+      <c r="J13">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F14" s="11"/>
+      <c r="G14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14">
+        <v>9000</v>
+      </c>
+      <c r="I14">
+        <v>120</v>
+      </c>
+      <c r="J14">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F15" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15">
+        <v>6000</v>
+      </c>
+      <c r="I15">
+        <v>80</v>
+      </c>
+      <c r="J15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F16" s="11"/>
+      <c r="G16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16">
+        <v>8000</v>
+      </c>
+      <c r="I16">
+        <v>120</v>
+      </c>
+      <c r="J16">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F17" s="11"/>
+      <c r="G17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17">
+        <v>10000</v>
+      </c>
+      <c r="I17">
+        <v>140</v>
+      </c>
+      <c r="J17">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="P21" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B22" s="6"/>
+      <c r="C22" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B23" s="6"/>
+      <c r="C23" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="N23" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B24" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="13">
+        <v>3</v>
+      </c>
+      <c r="D24" s="13">
+        <v>2</v>
+      </c>
+      <c r="E24" s="13">
+        <v>1</v>
+      </c>
+      <c r="F24" s="13">
+        <v>0</v>
+      </c>
+      <c r="G24" s="13">
+        <v>0</v>
+      </c>
+      <c r="H24" s="13">
+        <v>0</v>
+      </c>
+      <c r="I24" s="13">
+        <v>0</v>
+      </c>
+      <c r="J24" s="13">
+        <v>0</v>
+      </c>
+      <c r="K24" s="13">
+        <v>0</v>
+      </c>
+      <c r="L24" s="13">
+        <v>0</v>
+      </c>
+      <c r="M24" s="13">
+        <v>0</v>
+      </c>
+      <c r="N24" s="13">
+        <v>0</v>
+      </c>
+      <c r="O24" s="14">
+        <f>C24*$I$6+D24*$I$7+E24*$I$8+F24*$I$9+G24*$I$10+H24*$I$11+I24*$I$12+J24*$I$13+K24*$I$14+L24*$I$15+M24*$I$16+N24*$I$17</f>
+        <v>410</v>
+      </c>
+      <c r="P24" s="14">
+        <f>C24*$J$6+D24*$J$7+E24*$J$8+F24*$J$9+G24*$J$10+H24*$J$11+I24*$J$12+J24*$J$13+K24*$J$14+L24*$J$15+M24*$J$16+N24*$J$17</f>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B25" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="O25" s="14">
+        <f t="shared" ref="O25:O31" si="0">C25*$I$6+D25*$I$7+E25*$I$8+F25*$I$9+G25*$I$10+H25*$I$11+I25*$I$12+J25*$I$13+K25*$I$14+L25*$I$15+M25*$I$16+N25*$I$17</f>
+        <v>0</v>
+      </c>
+      <c r="P25" s="14">
+        <f t="shared" ref="P25:P31" si="1">C25*$J$6+D25*$J$7+E25*$J$8+F25*$J$9+G25*$J$10+H25*$J$11+I25*$J$12+J25*$J$13+K25*$J$14+L25*$J$15+M25*$J$16+N25*$J$17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B26" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O26" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P26" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B27" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="O27" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P27" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B28" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="O28" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P28" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B29" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="O29" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P29" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B30" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="O30" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P30" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="O31" s="14"/>
+      <c r="P31" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="O21:O23"/>
+    <mergeCell ref="P21:P23"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:K22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>